<commit_message>
criada função de adicionar alunos
</commit_message>
<xml_diff>
--- a/turma-2025-teste.xlsx
+++ b/turma-2025-teste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kauan\Documents\code\automacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC1EFF2-42F4-4F63-B79C-307F8ED3DCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B446D38-DC36-498D-A2C6-9315DC9564A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-45" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23775" yWindow="1680" windowWidth="15375" windowHeight="7875" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,20 +50,20 @@
     <t>Role</t>
   </si>
   <si>
-    <t>ricardo.ccorrea1@senacsp.edu.br</t>
-  </si>
-  <si>
-    <t>henri.cfernandes@senacsp.edu.br</t>
-  </si>
-  <si>
-    <t>paulo.cmmartins@senacsp.edu.br</t>
+    <t>teste.001@senacsp.edu.br</t>
+  </si>
+  <si>
+    <t>teste.002@senacsp.edu.br</t>
+  </si>
+  <si>
+    <t>teste.003@senacsp.edu.br</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -73,6 +73,14 @@
     <font>
       <b/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -95,14 +103,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -230,8 +241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -257,57 +268,63 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="str">
         <f t="shared" ref="B2:B4" si="0">A2</f>
-        <v>ricardo.ccorrea1@senacsp.edu.br</v>
+        <v>teste.001@senacsp.edu.br</v>
       </c>
       <c r="C2" t="str">
         <f>SUBSTITUTE(LEFT(A2, SEARCH("@", A2) - 1), ".", "_")</f>
-        <v>ricardo_ccorrea1</v>
+        <v>teste_001</v>
       </c>
       <c r="D2" t="str">
-        <f t="shared" ref="D2:D4" si="1">"TSC-2025-NOITE-" &amp; C2</f>
-        <v>TSC-2025-NOITE-ricardo_ccorrea1</v>
+        <f>"TSC-2025-TESTE-" &amp; C2</f>
+        <v>TSC-2025-TESTE-teste_001</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="str">
         <f t="shared" si="0"/>
-        <v>henri.cfernandes@senacsp.edu.br</v>
+        <v>teste.002@senacsp.edu.br</v>
       </c>
       <c r="C3" t="str">
         <f>SUBSTITUTE(LEFT(A3, SEARCH("@", A3) - 1), ".", "_")</f>
-        <v>henri_cfernandes</v>
+        <v>teste_002</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" si="1"/>
-        <v>TSC-2025-NOITE-henri_cfernandes</v>
+        <f t="shared" ref="D3:D4" si="1">"TSC-2025-TESTE-" &amp; C3</f>
+        <v>TSC-2025-TESTE-teste_002</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="str">
         <f t="shared" si="0"/>
-        <v>paulo.cmmartins@senacsp.edu.br</v>
+        <v>teste.003@senacsp.edu.br</v>
       </c>
       <c r="C4" t="str">
         <f>SUBSTITUTE(LEFT(A4, SEARCH("@", A4) - 1), ".", "_")</f>
-        <v>paulo_cmmartins</v>
+        <v>teste_003</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="1"/>
-        <v>TSC-2025-NOITE-paulo_cmmartins</v>
+        <v>TSC-2025-TESTE-teste_003</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{64129595-5F98-4F2E-856C-C5861E4E3B8E}"/>
+    <hyperlink ref="A3:A4" r:id="rId2" display="teste.001@senacsp.edu.br" xr:uid="{5BBB22BC-2360-4CA4-8B62-095002BC345C}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{A0911D91-9C63-4F4C-AD84-F851B740F4E4}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{3D66764B-9D59-460E-A589-E66F9BD46B6C}"/>
+  </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>